<commit_message>
Updated function lists referencing lddbd_core.php and lddbd_ajax.php to reflect correct line locations.
git-svn-id: http://plugins.svn.wordpress.org/ldd-business-directory/trunk@692488 b8457f37-d9ea-0310-8a92-e5e31aec5664
</commit_message>
<xml_diff>
--- a/ldd_businessdir_outline.xlsx
+++ b/ldd_businessdir_outline.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="130">
   <si>
     <t>lddbd_install()</t>
   </si>
@@ -107,12 +107,6 @@
     <t>FUNCTION/ROUTINE/VARIABLE</t>
   </si>
   <si>
-    <t>$lddbd_state_dropdown</t>
-  </si>
-  <si>
-    <t>A dropdown select list with all the states. Used in the Add/Edit Business pages(?).</t>
-  </si>
-  <si>
     <t>lddbd_setting_information_sections()</t>
   </si>
   <si>
@@ -1187,7 +1181,7 @@
     <t>Calls on the file that allows for WordPress functionality to be used.</t>
   </si>
   <si>
-    <t>148 to 150</t>
+    <t>95 to 97</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -1586,7 +1580,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>28</v>
@@ -1600,197 +1594,197 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>195</v>
+        <v>140</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>294</v>
+        <v>238</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>349</v>
+        <v>293</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>431</v>
+        <v>379</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>479</v>
+        <v>428</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>549</v>
+        <v>502</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>565</v>
+        <v>517</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>599</v>
+        <v>550</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>610</v>
+        <v>560</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>887</v>
+        <v>835</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>898</v>
+        <v>845</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>914</v>
+        <v>861</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1801,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,7 +1810,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>28</v>
@@ -1841,10 +1835,10 @@
         <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1852,10 +1846,10 @@
         <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1863,97 +1857,86 @@
         <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>35</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>89</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>55</v>
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>137</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>56</v>
+      <c r="A10" s="9">
+        <v>94</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>147</v>
+      <c r="A11" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>155</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="A12" s="1">
+        <v>102</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1979,7 +1962,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>28</v>
@@ -2092,16 +2075,16 @@
         <v>108</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2109,10 +2092,10 @@
         <v>160</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2120,10 +2103,10 @@
         <v>176</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,10 +2114,10 @@
         <v>191</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2158,7 +2141,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>28</v>
@@ -2172,22 +2155,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2195,10 +2178,10 @@
         <v>37</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2206,10 +2189,10 @@
         <v>193</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2217,28 +2200,28 @@
         <v>211</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2246,28 +2229,28 @@
         <v>451</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2275,10 +2258,10 @@
         <v>472</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2286,10 +2269,10 @@
         <v>473</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2297,10 +2280,10 @@
         <v>477</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
         <v>71</v>
-      </c>
-      <c r="C17" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2308,16 +2291,16 @@
         <v>754</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2341,7 +2324,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>28</v>
@@ -2355,10 +2338,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2366,10 +2349,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2377,10 +2360,10 @@
         <v>174</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2388,10 +2371,10 @@
         <v>198</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2399,10 +2382,10 @@
         <v>341</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2410,10 +2393,10 @@
         <v>385</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2421,10 +2404,10 @@
         <v>646</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>